<commit_message>
add modify result code
</commit_message>
<xml_diff>
--- a/TestCase/Baihe_Login.xlsx
+++ b/TestCase/Baihe_Login.xlsx
@@ -59,25 +59,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>http://plus.app.baihe.com/register/login?traceID=1&amp;systemID=2&amp;params={"mobile":"13716927954","password":"qqqqqqqq","appId":"1","plusPhoneModel":"Xiaomi-A1:C3 4W","plusChannel":"baihe_android_bhw_y","device":"864895021559263","appUpgradeVersionCode":76,"plusClientVersion":"7.4.0","apver":"7.4.0","plusCode":"0001","plusPhoneOSVersion":"4.4.4","plusPlatform":"1202","channel":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200,"msg":"","data":{"result":{"nickname":"\u9b41\u661f\u697c","headPhotoUrl":"http:\/\/photo5.baihe.com\/2016\/04\/18\/120_150\/2B99494BE2721548164FBC7BDAA5B1AD.jpg","gender":"1","age":29,"accountStatus":"1","marriage":"1","marriageChn":"\u672a\u5a5a","country":"86","countryChn":"\u4e2d\u56fd","province":"8611","provinceChn":"\u5317\u4eac\u5e02","city":"861113","cityChn":"\u5317\u4eac\u660c\u5e73","district":"861113","districtChn":"\u5317\u4eac\u660c\u5e73","income":"7","incomeChn":"10000-15000","isCreditedByAuth":"0","isCreditedById5":"0","isCreditedByMobile":"1","userService":170,"education":"5","educationChn":"\u672c\u79d1","height":"178","iFindOpPrefer":"10_01_01","prefer":"10_02_16,10_01_01,12_01_05,12_01_07,12_01_09,12_01_01,12_01_08,12_01_04,12_01_12,13_01_12","registerDate":"2015-08-05 14:24:45","longitude":"116.48127468533","latitude":"39.9960161675347","extra":"baihe","group_id":170,"birthday":"19880525","familyDescription":"\u672a\u5b9e\u540d\u8ba4\u8bc1\uff0c\u65e0\u7167\u7247\u8005\u52ff\u6270\u2026\u2026 ","hongdou":47,"photosNumber":"2","dataIntegrity":"98","hasMainPhoto":"1","userID":"124141212","match":{"matchEducation":"4,5,6,7,8","matchIncome":"5,6,7,8,9,10,11,12","matchHousing":"1,2,3,4,5,6,7,8","matchMarriage":"1","matchChildren":"1","matchMinAge":"18","matchMaxAge":"28","matchMinHeight":"160","matchMaxHeight":"168","matchCountry":"86","matchCountryChn":"\u4e2d\u56fd","matchProvince":"8611","matchProvinceChn":"\u5317\u4eac\u5e02","matchCity":"","matchCityChn":"","matchDistrict":"","matchDistrictChn":""},"housing":"3","housingChn":"\u79df\u623f","children":"1","childrenChn":"\u6ca1\u6709","loveType":"13","loveTypeChn":"\u827a\u672f\u5bb6\u578b","isCreditedBySesame":"0","headPhotoStatus":"1"},"other":0,"apver":"7.4.0"}}</t>
-  </si>
-  <si>
-    <t>http://plus.app.baihe.com/register/login?traceID=1&amp;systemID=2&amp;params={"mobile":"15198067024","password":"111111","appId":"1","plusPhoneModel":"Xiaomi-MI 4W","plusChannel":"baihe_android_bhw_y","device":"864895021559263","appUpgradeVersionCode":76,"plusClientVersion":"7.4.0","apver":"7.4.0","plusCode":"0001","plusPhoneOSVersion":"4.4.4","plusPlatform":"1202","channel":""}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"code":200,"msg":"","data":{"result":{"nickname":"\u963f\u72f8\u5230\u83b1\u5475\u5475","headPhotoUrl":"http:\/\/photo5.baihe.com\/2016\/03\/29\/120_150\/B05D51F18D35BC0F140D180A7ED5159D.jpg","gender":"0","age":30,"accountStatus":"1","marriage":"1","marriageChn":"\u672a\u5a5a","country":"86","countryChn":"\u4e2d\u56fd","province":"8611","provinceChn":"\u5317\u4eac\u5e02","city":"861101","cityChn":"\u5317\u4eac\u4e1c\u57ce","district":"861101","districtChn":"\u5317\u4eac\u4e1c\u57ce","income":"10","incomeChn":"25000-30000","isCreditedByAuth":"1","isCreditedById5":"1","isCreditedByMobile":"1","userService":98,"education":"3","educationChn":"\u9ad8\u4e2d","height":"180","iFindOpPrefer":"","prefer":"10_01_02,10_01_12,10_01_07,11_01_04,11_02_12,12_01_05,12_01_03,12_01_04,13_02_17","registerDate":"2015-10-14 15:01:26","longitude":"116.481271972656","latitude":"39.9960199652778","extra":"baihe","group_id":98,"birthday":"19871023","familyDescription":"\u65e0\u5b9e\u540d\u8ba4\u8bc1\uff0c\u65e0\u624b\u673a\u8ba4\u8bc1\uff0c\u65e0\u7167\u7247 \u52ff\u6270 \r\n\uff01\uff01\uff01\uff01\u5475\u5475\n\u83dc\u554a\u554a\u554a\n\u8c01\n\u662f\u8c01\n\u53c8\u662f\u8c01","hongdou":"","photosNumber":"0","dataIntegrity":"57","hasMainPhoto":"1","userID":"126784246","match":{"matchEducation":"1,2,3,4,5,6,7,8","matchIncome":"1,2,3,4,5,6,7,8","matchHousing":"1,2,3,4,5,6,7,8","matchMarriage":"1,2,3","matchChildren":"1,2,3,4","matchMinAge":"22","matchMaxAge":"44","matchMinHeight":"144","matchMaxHeight":"196","matchCountry":"86","matchCountryChn":"\u4e2d\u56fd","matchProvince":"8611","matchProvinceChn":"\u5317\u4eac\u5e02","matchCity":"","matchCityChn":"","matchDistrict":"","matchDistrictChn":""},"housing":"4","housingChn":"\u5df2\u8d2d\u623f(\u6709\u8d37\u6b3e)","children":"2","childrenChn":"\u6709\uff0c\u548c\u6211\u4f4f\u4e00\u8d77","loveType":"1","loveTypeChn":"\u54f2\u5b66\u5bb6\u578b","isCreditedBySesame":"0","headPhotoStatus":"1"},"other":0,"apver":"7.4.0"}}</t>
+    <t>http://plus.app.baihe.com/register/login?traceID=1&amp;systemID=2&amp;params={"mobile":"13716927954","password":"qqqqqqqq","appId":"1","plusPhoneModel":"Xiaomi-A1:C3 4W","plusChannel":"baihe_android_bhw_y","device":"864895021559263","appUpgradeVersionCode":76,"plusClientVersion":"7.4.0","apver":"7.6.0","plusCode":"0001","plusPhoneOSVersion":"4.4.4","plusPlatform":"1202","channel":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://plus.app.baihe.com/register/login?traceID=1&amp;systemID=2&amp;params={"mobile":"15198067024","password":"111111","appId":"1","plusPhoneModel":"Xiaomi-MI 4W","plusChannel":"baihe_android_bhw_y","device":"864895021559263","appUpgradeVersionCode":76,"plusClientVersion":"7.4.0","apver":"7.6.0","plusCode":"0001","plusPhoneOSVersion":"4.4.4","plusPlatform":"1202","channel":""}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200,"nickname":"阿狸到莱呵呵","apver":"7.6.0","gender":"0"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"code":200,"nickname":"果冻","apver":"7.6.0","gender":"1"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,14 +94,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -134,40 +128,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -499,11 +485,11 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="154" customHeight="1" x14ac:dyDescent="0.2">
@@ -513,19 +499,15 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C3" display="http://plus.app.baihe.com/register/login?traceID=1&amp;systemID=2&amp;params={&quot;mobile&quot;:&quot;13716927954&quot;,&quot;password&quot;:&quot;qqqqqqqq&quot;,&quot;appId&quot;:&quot;1&quot;,&quot;plusPhoneModel&quot;:&quot;Xiaomi-MI 4W&quot;,&quot;plusChannel&quot;:&quot;baihe_android_bhw_y&quot;,&quot;device&quot;:&quot;864895021559263&quot;,&quot;appUpgradeVersionCode&quot;:76,&quot;plusC"/>
-    <hyperlink ref="C2" display="http://plus.app.baihe.com/register/login?traceID=1&amp;systemID=2&amp;params={&quot;mobile&quot;:&quot;13716927954&quot;,&quot;password&quot;:&quot;qqqqqqqq&quot;,&quot;appId&quot;:&quot;1&quot;,&quot;plusPhoneModel&quot;:&quot;Xiaomi-MI 4W&quot;,&quot;plusChannel&quot;:&quot;baihe_android_bhw_y&quot;,&quot;device&quot;:&quot;864895021559263&quot;,&quot;appUpgradeVersionCode&quot;:76,&quot;plusC"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>